<commit_message>
Agreggated data from the old cbr site
</commit_message>
<xml_diff>
--- a/data/Dates of MP announcements by BoR.xlsx
+++ b/data/Dates of MP announcements by BoR.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\styrinka\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11832"/>
   </bookViews>
   <sheets>
     <sheet name="Dates of announcements" sheetId="1" r:id="rId1"/>
@@ -717,7 +717,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1143,17 +1143,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="36.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -1170,7 +1172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>40228</v>
       </c>
@@ -1187,7 +1189,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>40263</v>
       </c>
@@ -1204,7 +1206,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>40297</v>
       </c>
@@ -1221,7 +1223,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>40329</v>
       </c>
@@ -1238,7 +1240,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>40359</v>
       </c>
@@ -1255,7 +1257,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>40389</v>
       </c>
@@ -1272,7 +1274,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>40421</v>
       </c>
@@ -1289,7 +1291,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>40449</v>
       </c>
@@ -1306,7 +1308,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>40480</v>
       </c>
@@ -1323,7 +1325,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>40508</v>
       </c>
@@ -1340,7 +1342,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>40536</v>
       </c>
@@ -1357,7 +1359,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>40574</v>
       </c>
@@ -1374,7 +1376,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>40599</v>
       </c>
@@ -1391,7 +1393,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>40627</v>
       </c>
@@ -1408,7 +1410,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>40662</v>
       </c>
@@ -1425,7 +1427,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>40693</v>
       </c>
@@ -1442,7 +1444,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>40724</v>
       </c>
@@ -1459,7 +1461,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>40759</v>
       </c>
@@ -1476,7 +1478,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>40800</v>
       </c>
@@ -1493,7 +1495,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>40844</v>
       </c>
@@ -1510,7 +1512,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>40872</v>
       </c>
@@ -1527,7 +1529,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>40900</v>
       </c>
@@ -1544,7 +1546,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>40942</v>
       </c>
@@ -1561,7 +1563,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>40981</v>
       </c>
@@ -1578,7 +1580,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>41008</v>
       </c>
@@ -1595,7 +1597,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>41039</v>
       </c>
@@ -1612,7 +1614,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>41075</v>
       </c>
@@ -1629,7 +1631,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>41103</v>
       </c>
@@ -1646,7 +1648,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>41131</v>
       </c>
@@ -1663,7 +1665,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>41165</v>
       </c>
@@ -1680,7 +1682,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>41187</v>
       </c>
@@ -1697,7 +1699,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>41222</v>
       </c>
@@ -1714,7 +1716,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>41253</v>
       </c>
@@ -1731,7 +1733,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>41289</v>
       </c>
@@ -1748,7 +1750,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>41317</v>
       </c>
@@ -1765,7 +1767,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>41348</v>
       </c>
@@ -1782,7 +1784,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>41366</v>
       </c>
@@ -1799,7 +1801,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>41409</v>
       </c>
@@ -1816,7 +1818,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>41435</v>
       </c>
@@ -1833,7 +1835,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>41467</v>
       </c>
@@ -1850,7 +1852,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41495</v>
       </c>
@@ -1867,7 +1869,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>41530</v>
       </c>
@@ -1884,7 +1886,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>41561</v>
       </c>
@@ -1901,7 +1903,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>41586</v>
       </c>
@@ -1918,7 +1920,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>41621</v>
       </c>
@@ -1935,7 +1937,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>41684</v>
       </c>
@@ -1952,7 +1954,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>41701</v>
       </c>
@@ -1969,7 +1971,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>41712</v>
       </c>
@@ -1986,7 +1988,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>41754</v>
       </c>
@@ -2003,7 +2005,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>41806</v>
       </c>
@@ -2020,7 +2022,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>41845</v>
       </c>
@@ -2037,7 +2039,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>41894</v>
       </c>
@@ -2054,7 +2056,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>41943</v>
       </c>
@@ -2071,7 +2073,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>41984</v>
       </c>
@@ -2088,7 +2090,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>41989</v>
       </c>
@@ -2105,7 +2107,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>42034</v>
       </c>
@@ -2122,7 +2124,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>42076</v>
       </c>
@@ -2139,7 +2141,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>42124</v>
       </c>
@@ -2156,7 +2158,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>42170</v>
       </c>
@@ -2173,7 +2175,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>42216</v>
       </c>
@@ -2190,7 +2192,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>42258</v>
       </c>
@@ -2207,7 +2209,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>42307</v>
       </c>
@@ -2224,7 +2226,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>42349</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>42398</v>
       </c>
@@ -2258,7 +2260,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>42447</v>
       </c>
@@ -2275,7 +2277,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>42489</v>
       </c>
@@ -2292,7 +2294,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>42531</v>
       </c>
@@ -2309,7 +2311,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>42580</v>
       </c>
@@ -2326,7 +2328,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>42629</v>
       </c>
@@ -2343,7 +2345,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>42671</v>
       </c>
@@ -2360,7 +2362,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>42720</v>
       </c>
@@ -2377,7 +2379,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>42769</v>
       </c>
@@ -2394,7 +2396,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>42818</v>
       </c>
@@ -2411,7 +2413,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>42853</v>
       </c>
@@ -2428,7 +2430,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>42902</v>
       </c>
@@ -2445,7 +2447,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>42944</v>
       </c>
@@ -2462,7 +2464,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>42993</v>
       </c>
@@ -2479,7 +2481,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>43035</v>
       </c>
@@ -2496,7 +2498,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>43084</v>
       </c>
@@ -2513,7 +2515,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>43140</v>
       </c>
@@ -2530,7 +2532,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>43182</v>
       </c>
@@ -2547,7 +2549,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>43217</v>
       </c>
@@ -2564,7 +2566,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>43266</v>
       </c>
@@ -2581,7 +2583,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>43308</v>
       </c>
@@ -2598,7 +2600,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>43357</v>
       </c>
@@ -2615,7 +2617,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>43399</v>
       </c>
@@ -2632,7 +2634,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>43448</v>
       </c>
@@ -2649,7 +2651,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>43504</v>
       </c>
@@ -2666,7 +2668,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>43546</v>
       </c>
@@ -2683,7 +2685,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>43581</v>
       </c>
@@ -2700,7 +2702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>43630</v>
       </c>
@@ -2717,7 +2719,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>43672</v>
       </c>
@@ -2734,7 +2736,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>43714</v>
       </c>
@@ -2751,7 +2753,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>43763</v>
       </c>
@@ -2768,7 +2770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>43812</v>
       </c>
@@ -2785,7 +2787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>43868</v>
       </c>

</xml_diff>